<commit_message>
Update evaluation Excel files with new data
</commit_message>
<xml_diff>
--- a/eval_m_note.xlsx
+++ b/eval_m_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Polaris Office Sheet" lastEdited="7" lowestEdited="7" rupBuild="10.105.269.55310"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="590" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="580" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -303,7 +303,7 @@
       <color theme="1"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,6 +496,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -762,7 +768,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -792,6 +798,9 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -848,7 +857,7 @@
     <cellStyle name="통화" xfId="4" builtinId="4"/>
     <cellStyle name="통화[0]" xfId="7" builtinId="7"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -910,6 +919,26 @@
           <bgColor rgb="FFF8CBAD"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0095FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF8080"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0095FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF8080"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1190,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16.500000"/>
@@ -1215,7 +1244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="16.500000" hidden="1">
       <c r="A2" s="0" t="s">
         <v>15</v>
       </c>
@@ -1229,7 +1258,7 @@
         <v>0.947368421052631</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="16.500000" hidden="1">
       <c r="A3" s="0" t="s">
         <v>15</v>
       </c>
@@ -1243,7 +1272,7 @@
         <v>0.942583732057416</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="16.500000" hidden="1">
       <c r="A4" s="0" t="s">
         <v>15</v>
       </c>
@@ -1257,7 +1286,7 @@
         <v>0.937799043062201</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="16.500000" hidden="1">
       <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
@@ -1271,7 +1300,7 @@
         <v>0.937799043062201</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="16.500000" hidden="1">
       <c r="A6" s="0" t="s">
         <v>15</v>
       </c>
@@ -1285,7 +1314,7 @@
         <v>0.933014354066985</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="16.500000" hidden="1">
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
@@ -1299,7 +1328,7 @@
         <v>0.92822966507177</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="16.500000" hidden="1">
       <c r="A8" s="0" t="s">
         <v>15</v>
       </c>
@@ -1313,7 +1342,7 @@
         <v>0.92822966507177</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="16.500000" hidden="1">
       <c r="A9" s="0" t="s">
         <v>15</v>
       </c>
@@ -1327,7 +1356,7 @@
         <v>0.92822966507177</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="16.500000" hidden="1">
       <c r="A10" s="0" t="s">
         <v>15</v>
       </c>
@@ -1341,7 +1370,7 @@
         <v>0.923444976076555</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="16.500000" hidden="1">
       <c r="A11" s="0" t="s">
         <v>15</v>
       </c>
@@ -1355,7 +1384,7 @@
         <v>0.913875598086124</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="16.500000" hidden="1">
       <c r="A12" s="0" t="s">
         <v>16</v>
       </c>
@@ -1369,7 +1398,7 @@
         <v>0.977859778597786</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="16.500000" hidden="1">
       <c r="A13" s="0" t="s">
         <v>16</v>
       </c>
@@ -1383,7 +1412,7 @@
         <v>0.974169741697417</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="16.500000" hidden="1">
       <c r="A14" s="0" t="s">
         <v>16</v>
       </c>
@@ -1397,7 +1426,7 @@
         <v>0.974169741697417</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="16.500000" hidden="1">
       <c r="A15" s="0" t="s">
         <v>16</v>
       </c>
@@ -1411,7 +1440,7 @@
         <v>0.974169741697417</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="16.500000" hidden="1">
       <c r="A16" s="0" t="s">
         <v>16</v>
       </c>
@@ -1425,7 +1454,7 @@
         <v>0.974169741697417</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="16.500000" hidden="1">
       <c r="A17" s="0" t="s">
         <v>16</v>
       </c>
@@ -1439,7 +1468,7 @@
         <v>0.970479704797047</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="16.500000" hidden="1">
       <c r="A18" s="0" t="s">
         <v>16</v>
       </c>
@@ -1453,7 +1482,7 @@
         <v>0.970479704797047</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="16.500000" hidden="1">
       <c r="A19" s="0" t="s">
         <v>16</v>
       </c>
@@ -1467,7 +1496,7 @@
         <v>0.966789667896679</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="16.500000" hidden="1">
       <c r="A20" s="0" t="s">
         <v>16</v>
       </c>
@@ -1481,7 +1510,7 @@
         <v>0.963099630996309</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="16.500000" hidden="1">
       <c r="A21" s="0" t="s">
         <v>16</v>
       </c>
@@ -1495,7 +1524,7 @@
         <v>0.963099630996309</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="16.500000" hidden="1">
       <c r="A22" s="0" t="s">
         <v>17</v>
       </c>
@@ -1509,7 +1538,7 @@
         <v>0.950276243093922</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="16.500000" hidden="1">
       <c r="A23" s="0" t="s">
         <v>17</v>
       </c>
@@ -1523,7 +1552,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="16.500000" hidden="1">
       <c r="A24" s="0" t="s">
         <v>17</v>
       </c>
@@ -1537,7 +1566,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="16.500000" hidden="1">
       <c r="A25" s="0" t="s">
         <v>17</v>
       </c>
@@ -1551,7 +1580,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="16.500000" hidden="1">
       <c r="A26" s="0" t="s">
         <v>17</v>
       </c>
@@ -1565,7 +1594,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="16.500000" hidden="1">
       <c r="A27" s="0" t="s">
         <v>17</v>
       </c>
@@ -1579,7 +1608,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="16.500000" hidden="1">
       <c r="A28" s="0" t="s">
         <v>17</v>
       </c>
@@ -1593,7 +1622,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="16.500000" hidden="1">
       <c r="A29" s="0" t="s">
         <v>17</v>
       </c>
@@ -1607,7 +1636,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="16.500000" hidden="1">
       <c r="A30" s="0" t="s">
         <v>17</v>
       </c>
@@ -1621,7 +1650,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" ht="16.500000" hidden="1">
       <c r="A31" s="0" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1664,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" ht="16.500000" hidden="1">
       <c r="A32" s="0" t="s">
         <v>18</v>
       </c>
@@ -1649,7 +1678,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" ht="16.500000" hidden="1">
       <c r="A33" s="0" t="s">
         <v>18</v>
       </c>
@@ -1663,7 +1692,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="16.500000" hidden="1">
       <c r="A34" s="0" t="s">
         <v>18</v>
       </c>
@@ -1677,7 +1706,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="16.500000" hidden="1">
       <c r="A35" s="0" t="s">
         <v>18</v>
       </c>
@@ -1691,7 +1720,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="16.500000" hidden="1">
       <c r="A36" s="0" t="s">
         <v>18</v>
       </c>
@@ -1705,7 +1734,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" ht="16.500000" hidden="1">
       <c r="A37" s="0" t="s">
         <v>18</v>
       </c>
@@ -1719,7 +1748,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" ht="16.500000" hidden="1">
       <c r="A38" s="0" t="s">
         <v>18</v>
       </c>
@@ -1733,7 +1762,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" ht="16.500000" hidden="1">
       <c r="A39" s="0" t="s">
         <v>18</v>
       </c>
@@ -1747,7 +1776,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" ht="16.500000" hidden="1">
       <c r="A40" s="0" t="s">
         <v>18</v>
       </c>
@@ -1761,7 +1790,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" ht="16.500000" hidden="1">
       <c r="A41" s="0" t="s">
         <v>18</v>
       </c>
@@ -1775,7 +1804,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" ht="16.500000" hidden="1">
       <c r="A42" s="0" t="s">
         <v>19</v>
       </c>
@@ -1789,7 +1818,7 @@
         <v>0.917602996254681</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" ht="16.500000" hidden="1">
       <c r="A43" s="0" t="s">
         <v>19</v>
       </c>
@@ -1803,7 +1832,7 @@
         <v>0.910112359550561</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" ht="16.500000" hidden="1">
       <c r="A44" s="0" t="s">
         <v>19</v>
       </c>
@@ -1817,7 +1846,7 @@
         <v>0.906367041198501</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" ht="16.500000" hidden="1">
       <c r="A45" s="0" t="s">
         <v>19</v>
       </c>
@@ -1831,7 +1860,7 @@
         <v>0.902621722846441</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" ht="16.500000" hidden="1">
       <c r="A46" s="0" t="s">
         <v>19</v>
       </c>
@@ -1845,7 +1874,7 @@
         <v>0.902621722846441</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" ht="16.500000" hidden="1">
       <c r="A47" s="0" t="s">
         <v>19</v>
       </c>
@@ -1859,7 +1888,7 @@
         <v>0.902621722846441</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" ht="16.500000" hidden="1">
       <c r="A48" s="0" t="s">
         <v>19</v>
       </c>
@@ -1873,7 +1902,7 @@
         <v>0.898876404494382</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" ht="16.500000" hidden="1">
       <c r="A49" s="0" t="s">
         <v>19</v>
       </c>
@@ -1887,7 +1916,7 @@
         <v>0.898876404494382</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" ht="16.500000" hidden="1">
       <c r="A50" s="0" t="s">
         <v>19</v>
       </c>
@@ -1901,7 +1930,7 @@
         <v>0.895131086142322</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" ht="16.500000" hidden="1">
       <c r="A51" s="0" t="s">
         <v>19</v>
       </c>
@@ -1915,7 +1944,7 @@
         <v>0.891385767790262</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" ht="16.500000" hidden="1">
       <c r="A52" s="0" t="s">
         <v>20</v>
       </c>
@@ -1929,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" ht="16.500000" hidden="1">
       <c r="A53" s="0" t="s">
         <v>20</v>
       </c>
@@ -1943,7 +1972,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" ht="16.500000" hidden="1">
       <c r="A54" s="0" t="s">
         <v>20</v>
       </c>
@@ -1957,7 +1986,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" ht="16.500000" hidden="1">
       <c r="A55" s="0" t="s">
         <v>20</v>
       </c>
@@ -1971,7 +2000,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" ht="16.500000" hidden="1">
       <c r="A56" s="0" t="s">
         <v>20</v>
       </c>
@@ -1985,7 +2014,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" ht="16.500000" hidden="1">
       <c r="A57" s="0" t="s">
         <v>20</v>
       </c>
@@ -1999,7 +2028,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" ht="16.500000" hidden="1">
       <c r="A58" s="0" t="s">
         <v>20</v>
       </c>
@@ -2013,7 +2042,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" ht="16.500000" hidden="1">
       <c r="A59" s="0" t="s">
         <v>20</v>
       </c>
@@ -2027,7 +2056,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" ht="16.500000" hidden="1">
       <c r="A60" s="0" t="s">
         <v>20</v>
       </c>
@@ -2041,7 +2070,7 @@
         <v>0.988235294117647</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" ht="16.500000" hidden="1">
       <c r="A61" s="0" t="s">
         <v>20</v>
       </c>
@@ -2055,7 +2084,7 @@
         <v>0.988235294117647</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" ht="16.500000" hidden="1">
       <c r="A62" s="0" t="s">
         <v>21</v>
       </c>
@@ -2069,7 +2098,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" ht="16.500000" hidden="1">
       <c r="A63" s="0" t="s">
         <v>21</v>
       </c>
@@ -2083,7 +2112,7 @@
         <v>0.975</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" ht="16.500000" hidden="1">
       <c r="A64" s="0" t="s">
         <v>21</v>
       </c>
@@ -2097,7 +2126,7 @@
         <v>0.965</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" ht="16.500000" hidden="1">
       <c r="A65" s="0" t="s">
         <v>21</v>
       </c>
@@ -2111,7 +2140,7 @@
         <v>0.965</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" ht="16.500000" hidden="1">
       <c r="A66" s="0" t="s">
         <v>21</v>
       </c>
@@ -2125,7 +2154,7 @@
         <v>0.965</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" ht="16.500000" hidden="1">
       <c r="A67" s="0" t="s">
         <v>21</v>
       </c>
@@ -2139,7 +2168,7 @@
         <v>0.965</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" ht="16.500000" hidden="1">
       <c r="A68" s="0" t="s">
         <v>21</v>
       </c>
@@ -2153,7 +2182,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" ht="16.500000" hidden="1">
       <c r="A69" s="0" t="s">
         <v>21</v>
       </c>
@@ -2167,7 +2196,7 @@
         <v>0.955</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" ht="16.500000" hidden="1">
       <c r="A70" s="0" t="s">
         <v>21</v>
       </c>
@@ -2181,7 +2210,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" ht="16.500000" hidden="1">
       <c r="A71" s="0" t="s">
         <v>21</v>
       </c>
@@ -2195,7 +2224,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" ht="16.500000" hidden="1">
       <c r="A72" s="0" t="s">
         <v>22</v>
       </c>
@@ -2209,7 +2238,7 @@
         <v>0.942105263157894</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" ht="16.500000" hidden="1">
       <c r="A73" s="0" t="s">
         <v>22</v>
       </c>
@@ -2223,7 +2252,7 @@
         <v>0.936842105263157</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" ht="16.500000" hidden="1">
       <c r="A74" s="0" t="s">
         <v>22</v>
       </c>
@@ -2237,7 +2266,7 @@
         <v>0.931578947368421</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" ht="16.500000" hidden="1">
       <c r="A75" s="0" t="s">
         <v>22</v>
       </c>
@@ -2251,7 +2280,7 @@
         <v>0.931578947368421</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" ht="16.500000" hidden="1">
       <c r="A76" s="0" t="s">
         <v>22</v>
       </c>
@@ -2265,7 +2294,7 @@
         <v>0.926315789473684</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" ht="16.500000" hidden="1">
       <c r="A77" s="0" t="s">
         <v>22</v>
       </c>
@@ -2279,7 +2308,7 @@
         <v>0.926315789473684</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" ht="16.500000" hidden="1">
       <c r="A78" s="0" t="s">
         <v>22</v>
       </c>
@@ -2293,7 +2322,7 @@
         <v>0.926315789473684</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" ht="16.500000" hidden="1">
       <c r="A79" s="0" t="s">
         <v>22</v>
       </c>
@@ -2307,7 +2336,7 @@
         <v>0.926315789473684</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" ht="16.500000" hidden="1">
       <c r="A80" s="0" t="s">
         <v>22</v>
       </c>
@@ -2321,7 +2350,7 @@
         <v>0.921052631578947</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" ht="16.500000" hidden="1">
       <c r="A81" s="0" t="s">
         <v>22</v>
       </c>
@@ -2335,7 +2364,7 @@
         <v>0.910526315789473</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" ht="16.500000" hidden="1">
       <c r="A82" s="0" t="s">
         <v>23</v>
       </c>
@@ -2349,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" ht="16.500000" hidden="1">
       <c r="A83" s="0" t="s">
         <v>23</v>
       </c>
@@ -2363,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" ht="16.500000" hidden="1">
       <c r="A84" s="0" t="s">
         <v>23</v>
       </c>
@@ -2377,7 +2406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" ht="16.500000" hidden="1">
       <c r="A85" s="0" t="s">
         <v>23</v>
       </c>
@@ -2391,7 +2420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" ht="16.500000" hidden="1">
       <c r="A86" s="0" t="s">
         <v>23</v>
       </c>
@@ -2405,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" ht="16.500000" hidden="1">
       <c r="A87" s="0" t="s">
         <v>23</v>
       </c>
@@ -2419,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" ht="16.500000" hidden="1">
       <c r="A88" s="0" t="s">
         <v>23</v>
       </c>
@@ -2433,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" ht="16.500000" hidden="1">
       <c r="A89" s="0" t="s">
         <v>23</v>
       </c>
@@ -2447,7 +2476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" ht="16.500000" hidden="1">
       <c r="A90" s="0" t="s">
         <v>23</v>
       </c>
@@ -2461,7 +2490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" ht="16.500000" hidden="1">
       <c r="A91" s="0" t="s">
         <v>23</v>
       </c>
@@ -2475,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" ht="16.500000" hidden="1">
       <c r="A92" s="0" t="s">
         <v>24</v>
       </c>
@@ -2489,7 +2518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" ht="16.500000" hidden="1">
       <c r="A93" s="0" t="s">
         <v>24</v>
       </c>
@@ -2503,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" ht="16.500000" hidden="1">
       <c r="A94" s="0" t="s">
         <v>24</v>
       </c>
@@ -2517,7 +2546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" ht="16.500000" hidden="1">
       <c r="A95" s="0" t="s">
         <v>24</v>
       </c>
@@ -2531,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" ht="16.500000" hidden="1">
       <c r="A96" s="0" t="s">
         <v>24</v>
       </c>
@@ -2545,7 +2574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" ht="16.500000" hidden="1">
       <c r="A97" s="0" t="s">
         <v>24</v>
       </c>
@@ -2559,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" ht="16.500000" hidden="1">
       <c r="A98" s="0" t="s">
         <v>24</v>
       </c>
@@ -2573,7 +2602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" ht="16.500000" hidden="1">
       <c r="A99" s="0" t="s">
         <v>24</v>
       </c>
@@ -2587,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" ht="16.500000" hidden="1">
       <c r="A100" s="0" t="s">
         <v>24</v>
       </c>
@@ -2601,7 +2630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" ht="16.500000" hidden="1">
       <c r="A101" s="0" t="s">
         <v>24</v>
       </c>
@@ -2615,7 +2644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" ht="16.500000" hidden="1">
       <c r="A102" s="0" t="s">
         <v>25</v>
       </c>
@@ -2629,7 +2658,7 @@
         <v>0.920731707317073</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" ht="16.500000" hidden="1">
       <c r="A103" s="0" t="s">
         <v>25</v>
       </c>
@@ -2643,7 +2672,7 @@
         <v>0.908536585365853</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" ht="16.500000" hidden="1">
       <c r="A104" s="0" t="s">
         <v>25</v>
       </c>
@@ -2657,7 +2686,7 @@
         <v>0.908536585365853</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" ht="16.500000" hidden="1">
       <c r="A105" s="0" t="s">
         <v>25</v>
       </c>
@@ -2671,7 +2700,7 @@
         <v>0.908536585365853</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" ht="16.500000" hidden="1">
       <c r="A106" s="0" t="s">
         <v>25</v>
       </c>
@@ -2685,7 +2714,7 @@
         <v>0.902439024390243</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" ht="16.500000" hidden="1">
       <c r="A107" s="0" t="s">
         <v>25</v>
       </c>
@@ -2699,7 +2728,7 @@
         <v>0.896341463414634</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" ht="16.500000" hidden="1">
       <c r="A108" s="0" t="s">
         <v>25</v>
       </c>
@@ -2713,7 +2742,7 @@
         <v>0.896341463414634</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" ht="16.500000" hidden="1">
       <c r="A109" s="0" t="s">
         <v>25</v>
       </c>
@@ -2727,7 +2756,7 @@
         <v>0.890243902439024</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" ht="16.500000" hidden="1">
       <c r="A110" s="0" t="s">
         <v>25</v>
       </c>
@@ -2741,7 +2770,7 @@
         <v>0.878048780487804</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" ht="16.500000" hidden="1">
       <c r="A111" s="0" t="s">
         <v>25</v>
       </c>
@@ -2755,7 +2784,7 @@
         <v>0.871951219512195</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" ht="16.500000" hidden="1">
       <c r="A112" s="0" t="s">
         <v>26</v>
       </c>
@@ -2769,7 +2798,7 @@
         <v>0.964705882352941</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" ht="16.500000" hidden="1">
       <c r="A113" s="0" t="s">
         <v>26</v>
       </c>
@@ -2783,7 +2812,7 @@
         <v>0.958823529411764</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" ht="16.500000" hidden="1">
       <c r="A114" s="0" t="s">
         <v>26</v>
       </c>
@@ -2797,7 +2826,7 @@
         <v>0.952941176470588</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" ht="16.500000" hidden="1">
       <c r="A115" s="0" t="s">
         <v>26</v>
       </c>
@@ -2811,7 +2840,7 @@
         <v>0.947058823529411</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" ht="16.500000" hidden="1">
       <c r="A116" s="0" t="s">
         <v>26</v>
       </c>
@@ -2825,7 +2854,7 @@
         <v>0.941176470588235</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" ht="16.500000" hidden="1">
       <c r="A117" s="0" t="s">
         <v>26</v>
       </c>
@@ -2839,7 +2868,7 @@
         <v>0.941176470588235</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" ht="16.500000" hidden="1">
       <c r="A118" s="0" t="s">
         <v>26</v>
       </c>
@@ -2853,7 +2882,7 @@
         <v>0.935294117647058</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" ht="16.500000" hidden="1">
       <c r="A119" s="0" t="s">
         <v>26</v>
       </c>
@@ -2867,7 +2896,7 @@
         <v>0.935294117647058</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" ht="16.500000" hidden="1">
       <c r="A120" s="0" t="s">
         <v>26</v>
       </c>
@@ -2881,7 +2910,7 @@
         <v>0.923529411764705</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" ht="16.500000" hidden="1">
       <c r="A121" s="0" t="s">
         <v>26</v>
       </c>
@@ -2951,7 +2980,7 @@
         <v>0.866666666666666</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" ht="16.500000" hidden="1">
       <c r="A126" s="0" t="s">
         <v>27</v>
       </c>
@@ -2965,7 +2994,7 @@
         <v>0.866666666666666</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" ht="16.500000" hidden="1">
       <c r="A127" s="0" t="s">
         <v>27</v>
       </c>
@@ -3007,7 +3036,7 @@
         <v>0.861538461538461</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" ht="16.500000" hidden="1">
       <c r="A130" s="0" t="s">
         <v>27</v>
       </c>
@@ -3021,7 +3050,7 @@
         <v>0.856410256410256</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" ht="16.500000" hidden="1">
       <c r="A131" s="0" t="s">
         <v>27</v>
       </c>
@@ -3035,7 +3064,7 @@
         <v>0.851282051282051</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" ht="16.500000" hidden="1">
       <c r="A132" s="0" t="s">
         <v>38</v>
       </c>
@@ -3049,7 +3078,7 @@
         <v>0.977611940298507</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" ht="16.500000" hidden="1">
       <c r="A133" s="0" t="s">
         <v>38</v>
       </c>
@@ -3063,7 +3092,7 @@
         <v>0.977611940298507</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" ht="16.500000" hidden="1">
       <c r="A134" s="0" t="s">
         <v>38</v>
       </c>
@@ -3077,7 +3106,7 @@
         <v>0.973880597014925</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" ht="16.500000" hidden="1">
       <c r="A135" s="0" t="s">
         <v>38</v>
       </c>
@@ -3091,7 +3120,7 @@
         <v>0.973880597014925</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" ht="16.500000" hidden="1">
       <c r="A136" s="0" t="s">
         <v>38</v>
       </c>
@@ -3105,7 +3134,7 @@
         <v>0.970149253731343</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" ht="16.500000" hidden="1">
       <c r="A137" s="0" t="s">
         <v>38</v>
       </c>
@@ -3119,7 +3148,7 @@
         <v>0.970149253731343</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" ht="16.500000" hidden="1">
       <c r="A138" s="0" t="s">
         <v>38</v>
       </c>
@@ -3133,7 +3162,7 @@
         <v>0.970149253731343</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" ht="16.500000" hidden="1">
       <c r="A139" s="0" t="s">
         <v>38</v>
       </c>
@@ -3147,7 +3176,7 @@
         <v>0.973880597014925</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" ht="16.500000" hidden="1">
       <c r="A140" s="0" t="s">
         <v>38</v>
       </c>
@@ -3161,7 +3190,7 @@
         <v>0.973880597014925</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" ht="16.500000" hidden="1">
       <c r="A141" s="0" t="s">
         <v>38</v>
       </c>
@@ -3177,20 +3206,32 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D141">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="winograd(commonsense)"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="platinum_prompt"/>
+        <filter val="platinum_prompt_no_cot"/>
+        <filter val="RE2"/>
+        <filter val="RE2_no_cot"/>
+        <filter val="sRE2"/>
+        <filter val="sRE2_no_cot"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:D141">
       <sortCondition descending="1" ref="D2:D141"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="cot">
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="cot">
       <formula>NOT(ISERROR(SEARCH("cot",C1)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="9" priority="1" operator="notContains">
-      <formula>ISERROR(SEARCH("cot",$C$1))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="platinum_prompt">
-      <formula>NOT(ISERROR(SEARCH("platinum_prompt",C1)))</formula>
+    <cfRule type="notContainsText" dxfId="13" priority="1" operator="notContains">
+      <formula>ISERROR(SEARCH("no_cot",$C$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>

</xml_diff>